<commit_message>
POCE fix in shelf placement
</commit_message>
<xml_diff>
--- a/Projects/INBEVNL/Data/golden_shelves.xlsx
+++ b/Projects/INBEVNL/Data/golden_shelves.xlsx
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>num. of shelves min</t>
-  </si>
-  <si>
-    <t>num. of shelves max</t>
-  </si>
-  <si>
-    <t>num. ignored from top</t>
-  </si>
-  <si>
-    <t>num. ignored from bottom</t>
+    <t xml:space="preserve">num. of shelves min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num. of shelves max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num. ignored from top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num. ignored from bottom</t>
   </si>
 </sst>
 </file>
@@ -39,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -133,19 +133,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0728744939271"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3238866396761"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6437246963563"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.080971659919"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -190,35 +190,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>